<commit_message>
reduced mesh size and xlsx mod
</commit_message>
<xml_diff>
--- a/indexMap10x16.xlsx
+++ b/indexMap10x16.xlsx
@@ -1090,6 +1090,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1107,7 +1108,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,14 +1135,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCC66FF"/>
-        <bgColor rgb="FF9999FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor rgb="FFCC99FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1186,7 +1181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1208,10 +1203,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1240,7 +1231,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1263,8 +1254,8 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC66FF"/>
+      <rgbColor rgb="FFFF99FF"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -1295,7 +1286,7 @@
   <dimension ref="B12:W27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1860,28 +1851,28 @@
       <c r="D20" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="5" t="s">
         <v>186</v>
       </c>
       <c r="M20" s="4" t="s">
@@ -1940,19 +1931,19 @@
       <c r="H21" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="4" t="s">
         <v>209</v>
       </c>
       <c r="N21" s="4" t="s">
@@ -2008,19 +1999,19 @@
       <c r="H22" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="K22" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="L22" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="4" t="s">
         <v>231</v>
       </c>
       <c r="N22" s="4" t="s">
@@ -2076,19 +2067,19 @@
       <c r="H23" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="M23" s="4" t="s">
         <v>253</v>
       </c>
       <c r="N23" s="4" t="s">
@@ -2144,19 +2135,19 @@
       <c r="H24" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="J24" s="6" t="s">
+      <c r="J24" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="L24" s="6" t="s">
+      <c r="L24" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="4" t="s">
         <v>275</v>
       </c>
       <c r="N24" s="4" t="s">

</xml_diff>

<commit_message>
modified msh, and added pythonNoteBook
</commit_message>
<xml_diff>
--- a/indexMap10x16.xlsx
+++ b/indexMap10x16.xlsx
@@ -1085,7 +1085,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1107,8 +1107,14 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,13 +1124,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FFFF"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCFE7F5"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor rgb="FFFF99FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1136,7 +1148,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
-        <bgColor rgb="FFCC99FF"/>
+        <bgColor rgb="FFFF9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor rgb="FFFF9999"/>
       </patternFill>
     </fill>
   </fills>
@@ -1181,7 +1205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1203,6 +1227,42 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1238,7 +1298,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCFE7F5"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF66CC"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -1251,11 +1311,11 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FF99FFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF99FF99"/>
       <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF9999"/>
       <rgbColor rgb="FFFF99FF"/>
-      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -1283,10 +1343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B12:W27"/>
+  <dimension ref="B12:W37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T39" activeCellId="0" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1297,7 +1357,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +1425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1433,7 +1493,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
@@ -1501,7 +1561,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
         <v>66</v>
       </c>
@@ -1535,28 +1595,28 @@
       <c r="L15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="T15" s="4" t="s">
+      <c r="T15" s="5" t="s">
         <v>84</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -1569,7 +1629,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
         <v>88</v>
       </c>
@@ -1603,28 +1663,28 @@
       <c r="L16" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="P16" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="Q16" s="4" t="s">
+      <c r="Q16" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="S16" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="T16" s="5" t="s">
         <v>106</v>
       </c>
       <c r="U16" s="3" t="s">
@@ -1637,7 +1697,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
         <v>110</v>
       </c>
@@ -1671,28 +1731,28 @@
       <c r="L17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O17" s="4" t="s">
+      <c r="O17" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="P17" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="S17" s="4" t="s">
+      <c r="S17" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="T17" s="5" t="s">
         <v>128</v>
       </c>
       <c r="U17" s="3" t="s">
@@ -1705,7 +1765,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>132</v>
       </c>
@@ -1739,28 +1799,28 @@
       <c r="L18" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="O18" s="4" t="s">
+      <c r="O18" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="P18" s="4" t="s">
+      <c r="P18" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="Q18" s="4" t="s">
+      <c r="Q18" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="R18" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="S18" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="T18" s="4" t="s">
+      <c r="T18" s="5" t="s">
         <v>150</v>
       </c>
       <c r="U18" s="3" t="s">
@@ -1773,7 +1833,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>154</v>
       </c>
@@ -1807,28 +1867,28 @@
       <c r="L19" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="N19" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="O19" s="4" t="s">
+      <c r="O19" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="P19" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="Q19" s="4" t="s">
+      <c r="Q19" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="S19" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="T19" s="5" t="s">
         <v>172</v>
       </c>
       <c r="U19" s="3" t="s">
@@ -1841,7 +1901,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
         <v>176</v>
       </c>
@@ -1851,52 +1911,52 @@
       <c r="D20" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="N20" s="4" t="s">
+      <c r="N20" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="O20" s="4" t="s">
+      <c r="O20" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="P20" s="4" t="s">
+      <c r="P20" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="Q20" s="4" t="s">
+      <c r="Q20" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="R20" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="S20" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="T20" s="4" t="s">
+      <c r="T20" s="7" t="s">
         <v>194</v>
       </c>
       <c r="U20" s="3" t="s">
@@ -1909,7 +1969,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
         <v>198</v>
       </c>
@@ -1919,52 +1979,52 @@
       <c r="D21" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L21" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N21" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="O21" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="P21" s="4" t="s">
+      <c r="P21" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="Q21" s="4" t="s">
+      <c r="Q21" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="S21" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="T21" s="4" t="s">
+      <c r="T21" s="7" t="s">
         <v>216</v>
       </c>
       <c r="U21" s="3" t="s">
@@ -1977,7 +2037,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
         <v>220</v>
       </c>
@@ -1987,52 +2047,52 @@
       <c r="D22" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="N22" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="P22" s="4" t="s">
+      <c r="P22" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="Q22" s="4" t="s">
+      <c r="Q22" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="S22" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="T22" s="7" t="s">
         <v>238</v>
       </c>
       <c r="U22" s="3" t="s">
@@ -2045,7 +2105,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
         <v>242</v>
       </c>
@@ -2055,52 +2115,52 @@
       <c r="D23" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N23" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="O23" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="P23" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="R23" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="S23" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="T23" s="4" t="s">
+      <c r="T23" s="7" t="s">
         <v>260</v>
       </c>
       <c r="U23" s="3" t="s">
@@ -2113,7 +2173,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
         <v>264</v>
       </c>
@@ -2123,52 +2183,52 @@
       <c r="D24" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L24" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="N24" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="O24" s="4" t="s">
+      <c r="O24" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="P24" s="4" t="s">
+      <c r="P24" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="Q24" s="4" t="s">
+      <c r="Q24" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="R24" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="S24" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="T24" s="7" t="s">
         <v>282</v>
       </c>
       <c r="U24" s="3" t="s">
@@ -2181,7 +2241,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
         <v>286</v>
       </c>
@@ -2249,7 +2309,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
         <v>308</v>
       </c>
@@ -2317,7 +2377,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
         <v>330</v>
       </c>
@@ -2385,6 +2445,57 @@
         <v>351</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C33" s="8"/>
+      <c r="D33" s="9" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E33" s="9" t="n">
+        <v>-4</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C34" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D34" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C36" s="8"/>
+      <c r="D36" s="9" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E36" s="9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>